<commit_message>
feat: change logic to two termizators, update cleanings logic
</commit_message>
<xml_diff>
--- a/app/data/static/samples/by_department/rubber/sample_rubber_schedule.xlsx
+++ b/app/data/static/samples/by_department/rubber/sample_rubber_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Desktop/2024.04.19 терка мультиголовы/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Documents/coding/repos/nkrokhmal/umalat/app/data/static/samples/by_department/rubber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF86E9FE-49C9-1445-B60C-7699BA1F35D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56D82C0-7D07-464A-A00D-F5B1EE0526C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="780" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="файл остатки" sheetId="1" r:id="rId1"/>
@@ -1469,38 +1469,31 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -1550,37 +1543,18 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFEBF1DE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7A19A"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1629,6 +1603,32 @@
           <bgColor rgb="FFED1C24"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7A19A"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5595,10 +5595,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>295</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -5647,10 +5647,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="42" t="s">
         <v>299</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -5697,7 +5697,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="39"/>
-      <c r="B4" s="37"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="26" t="s">
         <v>302</v>
       </c>
@@ -5724,8 +5724,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="37" t="s">
         <v>295</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -5754,10 +5754,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>305</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -5804,7 +5804,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="27" t="s">
         <v>302</v>
       </c>
@@ -5831,8 +5831,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="41" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="38" t="s">
         <v>307</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -5861,10 +5861,10 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="42" t="s">
         <v>299</v>
       </c>
       <c r="C11" s="29" t="s">
@@ -6135,7 +6135,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="39"/>
-      <c r="B20" s="37"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="26" t="s">
         <v>314</v>
       </c>
@@ -6163,7 +6163,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="39"/>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="37" t="s">
         <v>295</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -6276,8 +6276,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="24" t="s">
         <v>317</v>
       </c>
@@ -6304,10 +6304,10 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="42" t="s">
         <v>299</v>
       </c>
       <c r="C28" s="29" t="s">
@@ -6550,7 +6550,7 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="39"/>
-      <c r="B36" s="37"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="26" t="s">
         <v>309</v>
       </c>
@@ -6578,7 +6578,7 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="39"/>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="37" t="s">
         <v>295</v>
       </c>
       <c r="C37" s="29" t="s">
@@ -6691,8 +6691,8 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="24" t="s">
         <v>303</v>
       </c>
@@ -6719,10 +6719,10 @@
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="43" t="s">
         <v>305</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -6769,7 +6769,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
-      <c r="B45" s="37"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="27" t="s">
         <v>302</v>
       </c>
@@ -6796,8 +6796,8 @@
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="41" t="s">
+      <c r="A46" s="40"/>
+      <c r="B46" s="38" t="s">
         <v>307</v>
       </c>
       <c r="C46" s="28" t="s">
@@ -6826,10 +6826,10 @@
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="43" t="s">
         <v>305</v>
       </c>
       <c r="C49" s="27" t="s">
@@ -7128,7 +7128,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="39"/>
-      <c r="B59" s="37"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="27" t="s">
         <v>317</v>
       </c>
@@ -7156,7 +7156,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="39"/>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="38" t="s">
         <v>307</v>
       </c>
       <c r="C60" s="28" t="s">
@@ -7409,8 +7409,8 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="40"/>
       <c r="C69" s="28" t="s">
         <v>328</v>
       </c>
@@ -7438,6 +7438,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B49:B59"/>
+    <mergeCell ref="B11:B20"/>
     <mergeCell ref="B2"/>
     <mergeCell ref="B60:B69"/>
     <mergeCell ref="A6:A8"/>
@@ -7454,10 +7458,6 @@
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="A28:A41"/>
     <mergeCell ref="B46"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B49:B59"/>
-    <mergeCell ref="B11:B20"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9018,7 +9018,7 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" ref="Q30:Q61" ca="1" si="13">IF(O30 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P30)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P30)))), 0)</f>
+        <f t="shared" ref="Q30:Q37" ca="1" si="13">IF(O30 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P30)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P30)))), 0)</f>
         <v>0</v>
       </c>
       <c r="R30">
@@ -10642,11 +10642,11 @@
       </c>
       <c r="M62" s="18"/>
       <c r="N62" s="17" t="str">
-        <f t="shared" ref="N62:N93" ca="1" si="22">IF(M62="", IF(X62=0, "", X62), IF(V62 = "", "", IF(V62/U62 = 0, "", V62/U62)))</f>
+        <f t="shared" ref="N62:N86" ca="1" si="22">IF(M62="", IF(X62=0, "", X62), IF(V62 = "", "", IF(V62/U62 = 0, "", V62/U62)))</f>
         <v/>
       </c>
       <c r="P62">
-        <f t="shared" ref="P62:P93" si="23">IF(O62 = "-", -W62,I62)</f>
+        <f t="shared" ref="P62:P86" si="23">IF(O62 = "-", -W62,I62)</f>
         <v>0</v>
       </c>
       <c r="Q62">
@@ -10674,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="W62">
-        <f t="shared" ref="W62:W93" ca="1" si="28">IF(V62 = "", "", V62/U62)</f>
+        <f t="shared" ref="W62:W86" ca="1" si="28">IF(V62 = "", "", V62/U62)</f>
         <v>0</v>
       </c>
       <c r="X62" t="str">
@@ -12635,23 +12635,23 @@
       <formula>$B2&lt;&gt;$T2</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>SUMIF(J2:J86,"&gt;0")-SUMIF(J2:J86,"&lt;0") &gt; 1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>IF(N1="",0, J1)  &lt; - 0.05* IF(N1="",0,N1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>AND(IF(N1="",0, J1)  &gt;= - 0.05* IF(N1="",0,N1), IF(N1="",0, J1) &lt; 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>AND(IF(N1="",0, J1)  &lt;= 0.05* IF(N1="",0,N1), IF(N1="",0, J1) &gt; 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>IF(N1="",0,J1)  &gt; 0.05* IF(N1="",0,N1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="expression" dxfId="6" priority="11">
-      <formula>SUMIF(J2:J86,"&gt;0")-SUMIF(J2:J86,"&lt;0") &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -12705,8 +12705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5924EC5-9E1A-164C-8C52-1A3606F449D7}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12718,7 +12718,7 @@
       <c r="A1" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="36" t="s">
         <v>336</v>
       </c>
     </row>
@@ -12939,7 +12939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
@@ -14319,11 +14319,11 @@
       </c>
       <c r="M21" s="18"/>
       <c r="N21" s="17" t="str">
-        <f t="shared" ref="N21:N52" ca="1" si="20">IF(M21="", IF(X21=0, "", X21), IF(V21 = "", "", IF(V21/U21 = 0, "", V21/U21)))</f>
+        <f t="shared" ref="N21:N45" ca="1" si="20">IF(M21="", IF(X21=0, "", X21), IF(V21 = "", "", IF(V21/U21 = 0, "", V21/U21)))</f>
         <v/>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P52" si="21">IF(O21 = "-", -W21,I21)</f>
+        <f t="shared" ref="P21:P45" si="21">IF(O21 = "-", -W21,I21)</f>
         <v>0</v>
       </c>
       <c r="Q21">
@@ -14351,7 +14351,7 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <f t="shared" ref="W21:W52" ca="1" si="26">IF(V21 = "", "", V21/U21)</f>
+        <f t="shared" ref="W21:W45" ca="1" si="26">IF(V21 = "", "", V21/U21)</f>
         <v>0</v>
       </c>
       <c r="X21" t="str">
@@ -17031,23 +17031,23 @@
       <formula>$B2&lt;&gt;$T2</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="expression" dxfId="4" priority="29">
+      <formula>SUMIF(J2:J45,"&gt;0")-SUMIF(J2:J45,"&lt;0") &gt; 1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF(N1="",0, J1)  &lt; - 0.05* IF(N1="",0,N1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND(IF(N1="",0, J1)  &gt;= - 0.05* IF(N1="",0,N1), IF(N1="",0, J1) &lt; 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>IF(N1="",0,J1)  &gt; 0.05* IF(N1="",0,N1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>AND(IF(N1="",0, J1)  &lt;= 0.05* IF(N1="",0,N1), IF(N1="",0, J1) &gt; 0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="expression" dxfId="0" priority="29">
-      <formula>SUMIF(J2:J45,"&gt;0")-SUMIF(J2:J45,"&lt;0") &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>